<commit_message>
fixed #27 #28 mmlLs:Lifestyle module
</commit_message>
<xml_diff>
--- a/mapping/mml_lifestyle_mapping.xlsx
+++ b/mapping/mml_lifestyle_mapping.xlsx
@@ -16,16 +16,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
   <si>
     <t>mmlLs:LifestyleModule</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>mml_lifestyle</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>mmlLs:occupation</t>
   </si>
   <si>
@@ -35,46 +31,14 @@
     <t>mmlLs:alcohol</t>
   </si>
   <si>
-    <t>mmlLs:other</t>
-  </si>
-  <si>
     <t>Archetype</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>element</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Exposed risk from occupation</t>
-  </si>
-  <si>
     <t>path</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Tobacco Use Summary</t>
-  </si>
-  <si>
-    <t>/data/Usage status</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Alcohol Use Summary</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Other substance use summary</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>/data/Overall Description</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>/content[openEHR-EHR-EVALUATION.exposure.v1 and name/value='Exposed risk from occupation']/data[at0001]/items[at0003]</t>
-  </si>
-  <si>
     <t>/content[openEHR-EHR-EVALUATION.substance_use_summary-tobacco.v1 and name/value='Tobacco Use Summary']/data[at0001]/items[at0002]</t>
   </si>
   <si>
@@ -84,29 +48,82 @@
     <t>/content[openEHR-EHR-EVALUATION.substance_use_summary.v1 and name/value='Other Substance Use Summary']/data[at0001]/items[at0002]</t>
   </si>
   <si>
-    <t>生活歴モジュール</t>
-    <rPh sb="0" eb="2">
-      <t>セイカツ</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>レキ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>occurrence</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>必ず1回出現</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>必ず1回出現</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>0回もしくは1回出現</t>
+    <t>Elements　</t>
+  </si>
+  <si>
+    <t>Attribute</t>
+  </si>
+  <si>
+    <t>Datatypes</t>
+  </si>
+  <si>
+    <t>Occurrence</t>
+  </si>
+  <si>
+    <t>Table id</t>
+  </si>
+  <si>
+    <t>mmlLs:LifestyleModule</t>
+  </si>
+  <si>
+    <t>1.1.</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>1.2.</t>
+  </si>
+  <si>
+    <t>1.3.</t>
+  </si>
+  <si>
+    <t>1.4.</t>
+  </si>
+  <si>
+    <t>mmlLs:other　</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>MML</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>node</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>openEHR-EHR-EVALUATION.exposure.v1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-EVALUATION.exposure.v1 and name/value='Exposed risk from occupation']/data[at0001]/items[at0010 and name/value='Exposure Details']/items[at0013]</t>
+  </si>
+  <si>
+    <t>exposure details/Description</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>openEHR-EHR-COMPOSITION.lifestyle_factors.v1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>openEHR-EHR-EVALUATION.substance_use_summary-tobacco.v1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>usage status</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>openEHR-EHR-EVALUATION.substance_use_summary-alcohol.v1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>openEHR-EHR-EVALUATION.substance_use_summary.v1</t>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
@@ -146,12 +163,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -160,7 +192,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -169,6 +201,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -471,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -483,104 +518,156 @@
     <col min="2" max="2" width="20.25" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="53.375" customWidth="1"/>
+    <col min="9" max="9" width="18.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="H2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="27" x14ac:dyDescent="0.15">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A4" s="3">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="H4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="H5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="H6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="H7" t="s">
+        <v>30</v>
+      </c>
+      <c r="I7" t="s">
+        <v>29</v>
+      </c>
+      <c r="J7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="B8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="B2" s="2"/>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="B3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="C8" s="3"/>
+      <c r="D8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F8" s="3"/>
+      <c r="H8" t="s">
+        <v>31</v>
+      </c>
+      <c r="I8" t="s">
+        <v>29</v>
+      </c>
+      <c r="J8" t="s">
         <v>8</v>
       </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="B4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="B5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="B6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="B7" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>